<commit_message>
Start revision from windows side
</commit_message>
<xml_diff>
--- a/publication/supplement_tables/supplementary_tables.xlsx
+++ b/publication/supplement_tables/supplementary_tables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\felix\Desktop\rodent_loss\publication\supplement_tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{323D0136-3144-428E-BF45-1B3087801494}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B272EBD2-B09A-4E06-85EE-5B80449649A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-18120" windowWidth="29040" windowHeight="17520" firstSheet="4" activeTab="8" xr2:uid="{5E6BDF8B-5678-42D7-A593-A9BF15DF20B3}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="5" activeTab="6" xr2:uid="{5E6BDF8B-5678-42D7-A593-A9BF15DF20B3}"/>
   </bookViews>
   <sheets>
     <sheet name="S1_miRNA_overview" sheetId="1" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6680" uniqueCount="1808">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6682" uniqueCount="1810">
   <si>
     <t>miRNA family</t>
   </si>
@@ -5471,6 +5471,12 @@
   </si>
   <si>
     <t xml:space="preserve">Table S9. Phylostrata of human transcription factors and determination of core transcription factors. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">To identify core TFs, we first determined the minimum age of each TF by finding the LCA of the two most diverged species for which an ortholog was found. We then compared the number of species with an ortholog to the number of taxa subsumed under the respective LCA. To account for noise in the phylogenetic profiles, we allowed core-TFs to be absent in 5% of the taxa </t>
+  </si>
+  <si>
+    <t>Is MirTarBase target</t>
   </si>
 </sst>
 </file>
@@ -5531,18 +5537,31 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="3">
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -5560,20 +5579,6 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-      </border>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -5603,7 +5608,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{EF655A70-172A-4CE7-9174-546481342A61}" name="Table2" displayName="Table2" ref="A2:J89" totalsRowShown="0" headerRowDxfId="0" headerRowBorderDxfId="1" tableBorderDxfId="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{EF655A70-172A-4CE7-9174-546481342A61}" name="Table2" displayName="Table2" ref="A2:J89" totalsRowShown="0" headerRowDxfId="2" headerRowBorderDxfId="1" tableBorderDxfId="0">
   <autoFilter ref="A2:J89" xr:uid="{EF655A70-172A-4CE7-9174-546481342A61}"/>
   <tableColumns count="10">
     <tableColumn id="1" xr3:uid="{4D2302F3-DBF5-4069-9AE1-AD1723F7C88C}" name="miRTarBase ID"/>
@@ -5689,10 +5694,11 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{D2A1260B-28C5-4D58-ACB8-A432A535FC24}" name="Table14" displayName="Table14" ref="A2:A130" totalsRowShown="0">
-  <autoFilter ref="A2:A130" xr:uid="{D2A1260B-28C5-4D58-ACB8-A432A535FC24}"/>
-  <tableColumns count="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{D2A1260B-28C5-4D58-ACB8-A432A535FC24}" name="Table14" displayName="Table14" ref="A2:B130" totalsRowShown="0">
+  <autoFilter ref="A2:B130" xr:uid="{D2A1260B-28C5-4D58-ACB8-A432A535FC24}"/>
+  <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{052BAD53-01BA-49F6-80B9-337D91B1FFFC}" name="Symbol"/>
+    <tableColumn id="2" xr3:uid="{5B325C03-E98A-4464-922E-D996D8C34888}" name="Is MirTarBase target"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -6055,296 +6061,296 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.4">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="4" t="s">
         <v>1799</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="4" t="s">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="4" t="s">
+      <c r="A3" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="4">
-        <v>1</v>
-      </c>
-      <c r="D3" s="4">
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
         <v>18</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="4" t="s">
+      <c r="A4" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="4">
-        <v>1</v>
-      </c>
-      <c r="D4" s="4">
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
         <v>18</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="4" t="s">
+      <c r="A5" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="4">
-        <v>1</v>
-      </c>
-      <c r="D5" s="4">
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
         <v>23</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E5" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" s="4" t="s">
+      <c r="A6" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="4">
-        <v>1</v>
-      </c>
-      <c r="D6" s="4">
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
         <v>25</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="E6" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" s="4" t="s">
+      <c r="A7" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="4">
-        <v>1</v>
-      </c>
-      <c r="D7" s="4">
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
         <v>29</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="E7" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" s="4" t="s">
+      <c r="A8" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="4">
+      <c r="C8">
         <v>20</v>
       </c>
-      <c r="D8" s="4">
+      <c r="D8">
         <v>34</v>
       </c>
-      <c r="E8" s="4" t="s">
+      <c r="E8" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" s="4" t="s">
+      <c r="A9" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="4">
-        <v>1</v>
-      </c>
-      <c r="D9" s="4">
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9">
         <v>36</v>
       </c>
-      <c r="E9" s="4" t="s">
+      <c r="E9" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" s="4" t="s">
+      <c r="A10" t="s">
         <v>21</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="4">
-        <v>1</v>
-      </c>
-      <c r="D10" s="4">
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10">
         <v>36</v>
       </c>
-      <c r="E10" s="4" t="s">
+      <c r="E10" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" s="4" t="s">
+      <c r="A11" t="s">
         <v>23</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" t="s">
         <v>6</v>
       </c>
-      <c r="C11" s="4">
-        <v>1</v>
-      </c>
-      <c r="D11" s="4">
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11">
         <v>38</v>
       </c>
-      <c r="E11" s="4" t="s">
+      <c r="E11" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" s="4" t="s">
+      <c r="A12" t="s">
         <v>25</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" t="s">
         <v>6</v>
       </c>
-      <c r="C12" s="4">
-        <v>1</v>
-      </c>
-      <c r="D12" s="4">
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12">
         <v>39</v>
       </c>
-      <c r="E12" s="4" t="s">
+      <c r="E12" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" s="4" t="s">
+      <c r="A13" t="s">
         <v>27</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B13" t="s">
         <v>6</v>
       </c>
-      <c r="C13" s="4">
-        <v>1</v>
-      </c>
-      <c r="D13" s="4">
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13">
         <v>44</v>
       </c>
-      <c r="E13" s="4" t="s">
+      <c r="E13" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="25.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="4" t="s">
+      <c r="A14" t="s">
         <v>29</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B14" t="s">
         <v>30</v>
       </c>
-      <c r="C14" s="4">
+      <c r="C14">
         <v>2</v>
       </c>
-      <c r="D14" s="4">
+      <c r="D14">
         <v>48</v>
       </c>
-      <c r="E14" s="4" t="s">
+      <c r="E14" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" s="4" t="s">
+      <c r="A15" t="s">
         <v>32</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B15" t="s">
         <v>6</v>
       </c>
-      <c r="C15" s="4">
-        <v>1</v>
-      </c>
-      <c r="D15" s="4">
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15">
         <v>52</v>
       </c>
-      <c r="E15" s="4" t="s">
+      <c r="E15" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16" s="4" t="s">
+      <c r="A16" t="s">
         <v>34</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="B16" t="s">
         <v>6</v>
       </c>
-      <c r="C16" s="4">
-        <v>1</v>
-      </c>
-      <c r="D16" s="4">
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16">
         <v>59</v>
       </c>
-      <c r="E16" s="4" t="s">
+      <c r="E16" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" s="4" t="s">
+      <c r="A17" t="s">
         <v>36</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="B17" t="s">
         <v>6</v>
       </c>
-      <c r="C17" s="4">
-        <v>1</v>
-      </c>
-      <c r="D17" s="4">
+      <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="D17">
         <v>64</v>
       </c>
-      <c r="E17" s="4" t="s">
+      <c r="E17" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" s="4" t="s">
+      <c r="A18" t="s">
         <v>38</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="B18" t="s">
         <v>6</v>
       </c>
-      <c r="C18" s="4">
-        <v>1</v>
-      </c>
-      <c r="D18" s="4">
+      <c r="C18">
+        <v>1</v>
+      </c>
+      <c r="D18">
         <v>67</v>
       </c>
-      <c r="E18" s="4" t="s">
+      <c r="E18" t="s">
         <v>39</v>
       </c>
     </row>
@@ -6378,7 +6384,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="21" x14ac:dyDescent="0.4">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="4" t="s">
         <v>1800</v>
       </c>
     </row>
@@ -9222,7 +9228,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="21" x14ac:dyDescent="0.4">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="4" t="s">
         <v>1801</v>
       </c>
     </row>
@@ -32910,7 +32916,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD88AEBC-F68A-461A-A083-8A23868FF8C0}">
   <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -32919,7 +32927,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.4">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="4" t="s">
         <v>1802</v>
       </c>
     </row>
@@ -33407,7 +33415,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="21" x14ac:dyDescent="0.4">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="4" t="s">
         <v>1803</v>
       </c>
     </row>
@@ -42768,7 +42776,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.4">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="4" t="s">
         <v>1804</v>
       </c>
     </row>
@@ -42901,658 +42909,1044 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4EA71B4E-7288-44D8-81FF-D12D41C6D403}">
-  <dimension ref="A1:A129"/>
+  <dimension ref="A1:B129"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A105" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:B129"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="10.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="21" x14ac:dyDescent="0.4">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:2" ht="21" x14ac:dyDescent="0.4">
+      <c r="A1" s="4" t="s">
         <v>1805</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1798</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>1809</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>862</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>863</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>864</v>
       </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B5" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>865</v>
       </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>866</v>
       </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>867</v>
       </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B8" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>852</v>
       </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B9" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>868</v>
       </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B10" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>869</v>
       </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B11" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>870</v>
       </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B12" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>871</v>
       </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B13" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>872</v>
       </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B14" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>873</v>
       </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>874</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B16" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>875</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B17" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>876</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B18" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>877</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B19" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>878</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B20" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>879</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B21" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>880</v>
       </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B22" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>881</v>
       </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B23" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>882</v>
       </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B24" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>883</v>
       </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B25" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>884</v>
       </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B26" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>885</v>
       </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B27" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>886</v>
       </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B28" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>887</v>
       </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>888</v>
       </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B30" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>889</v>
       </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B31" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>890</v>
       </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B32" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>891</v>
       </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B33" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>829</v>
       </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B34" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>892</v>
       </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B35" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>893</v>
       </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B36" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>894</v>
       </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B37" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>895</v>
       </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B38" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>896</v>
       </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B39" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>897</v>
       </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B40" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>898</v>
       </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B41" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>899</v>
       </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B42" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>855</v>
       </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B43" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>900</v>
       </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B44" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>901</v>
       </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B45" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>902</v>
       </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B46" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>903</v>
       </c>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B47" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>904</v>
       </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B48" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>905</v>
       </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B49" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>906</v>
       </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B50" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>907</v>
       </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B51" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>908</v>
       </c>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B52" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>909</v>
       </c>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B53" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>910</v>
       </c>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B54" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>911</v>
       </c>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B55" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>912</v>
       </c>
-    </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B56" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>913</v>
       </c>
-    </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B57" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>914</v>
       </c>
-    </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B58" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>915</v>
       </c>
-    </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B59" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>916</v>
       </c>
-    </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B60" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>917</v>
       </c>
-    </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B61" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>918</v>
       </c>
-    </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B62" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>919</v>
       </c>
-    </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B63" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>920</v>
       </c>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B64" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>921</v>
       </c>
-    </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B65" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>922</v>
       </c>
-    </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B66" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>923</v>
       </c>
-    </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B67" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>924</v>
       </c>
-    </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B68" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>857</v>
       </c>
-    </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B69" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>925</v>
       </c>
-    </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B70" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>926</v>
       </c>
-    </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B71" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>927</v>
       </c>
-    </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B72" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>928</v>
       </c>
-    </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B73" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>929</v>
       </c>
-    </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B74" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>930</v>
       </c>
-    </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B75" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>931</v>
       </c>
-    </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B76" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>932</v>
       </c>
-    </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B77" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>933</v>
       </c>
-    </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B78" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>934</v>
       </c>
-    </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B79" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>935</v>
       </c>
-    </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B80" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>936</v>
       </c>
-    </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B81" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>847</v>
       </c>
-    </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B82" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>937</v>
       </c>
-    </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B83" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>938</v>
       </c>
-    </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B84" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>939</v>
       </c>
-    </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B85" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>940</v>
       </c>
-    </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B86" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>941</v>
       </c>
-    </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B87" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>942</v>
       </c>
-    </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B88" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>943</v>
       </c>
-    </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B89" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>944</v>
       </c>
-    </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B90" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>945</v>
       </c>
-    </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B91" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>946</v>
       </c>
-    </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B92" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>947</v>
       </c>
-    </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B93" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>948</v>
       </c>
-    </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B94" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>949</v>
       </c>
-    </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B95" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>950</v>
       </c>
-    </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B96" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>951</v>
       </c>
-    </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B97" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>952</v>
       </c>
-    </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B98" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>953</v>
       </c>
-    </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B99" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>954</v>
       </c>
-    </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B100" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>955</v>
       </c>
-    </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B101" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>956</v>
       </c>
-    </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B102" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>957</v>
       </c>
-    </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B103" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>958</v>
       </c>
-    </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B104" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>959</v>
       </c>
-    </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B105" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>960</v>
       </c>
-    </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B106" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>961</v>
       </c>
-    </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B107" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>962</v>
       </c>
-    </row>
-    <row r="109" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B108" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>963</v>
       </c>
-    </row>
-    <row r="110" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B109" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>964</v>
       </c>
-    </row>
-    <row r="111" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B110" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>965</v>
       </c>
-    </row>
-    <row r="112" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B111" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>966</v>
       </c>
-    </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B112" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>967</v>
       </c>
-    </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B113" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>968</v>
       </c>
-    </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B114" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>969</v>
       </c>
-    </row>
-    <row r="116" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B115" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>970</v>
       </c>
-    </row>
-    <row r="117" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B116" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>971</v>
       </c>
-    </row>
-    <row r="118" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B117" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>972</v>
       </c>
-    </row>
-    <row r="119" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B118" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>973</v>
       </c>
-    </row>
-    <row r="120" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B119" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
         <v>974</v>
       </c>
-    </row>
-    <row r="121" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B120" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
         <v>975</v>
       </c>
-    </row>
-    <row r="122" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B121" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
         <v>831</v>
       </c>
-    </row>
-    <row r="123" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B122" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
         <v>976</v>
       </c>
-    </row>
-    <row r="124" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B123" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
         <v>844</v>
       </c>
-    </row>
-    <row r="125" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B124" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
         <v>977</v>
       </c>
-    </row>
-    <row r="126" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B125" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
         <v>978</v>
       </c>
-    </row>
-    <row r="127" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B126" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
         <v>979</v>
       </c>
-    </row>
-    <row r="128" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B127" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
         <v>980</v>
       </c>
-    </row>
-    <row r="129" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B128" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
         <v>981</v>
+      </c>
+      <c r="B129" t="b">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -43575,7 +43969,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.4">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="4" t="s">
         <v>1806</v>
       </c>
     </row>
@@ -43771,9 +44165,11 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6A8B04A-7617-4C23-AFE3-CAA38D40B75E}">
-  <dimension ref="A1:G1606"/>
+  <dimension ref="A1:J1606"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -43785,12 +44181,15 @@
     <col min="6" max="6" width="25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="21" x14ac:dyDescent="0.4">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:10" ht="21" x14ac:dyDescent="0.4">
+      <c r="A1" s="4" t="s">
         <v>1807</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="J1" t="s">
+        <v>1808</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1797</v>
       </c>
@@ -43811,7 +44210,7 @@
       </c>
       <c r="G2" s="2"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1790</v>
       </c>
@@ -43831,7 +44230,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>1790</v>
       </c>
@@ -43851,7 +44250,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>1790</v>
       </c>
@@ -43871,7 +44270,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -43891,7 +44290,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>1790</v>
       </c>
@@ -43911,7 +44310,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>1790</v>
       </c>
@@ -43931,7 +44330,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>1790</v>
       </c>
@@ -43951,7 +44350,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>15</v>
       </c>
@@ -43971,7 +44370,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>1790</v>
       </c>
@@ -43991,7 +44390,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>1790</v>
       </c>
@@ -44011,7 +44410,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>1790</v>
       </c>
@@ -44031,7 +44430,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -44051,7 +44450,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>6</v>
       </c>
@@ -44071,7 +44470,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>15</v>
       </c>

</xml_diff>